<commit_message>
letter A for Green
</commit_message>
<xml_diff>
--- a/Green Function Method/pattern_code_far_field.xlsx
+++ b/Green Function Method/pattern_code_far_field.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Non-Hermitian Gauge Field\non-hermitian-gauge-field\Green Function Method\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAF5E09-A255-433E-96A0-B1266EE0242F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89E43DB-B7B0-442D-A7E0-720C8D0703B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="852" yWindow="-108" windowWidth="22296" windowHeight="13176" activeTab="1" xr2:uid="{F0408D6B-1B69-4349-BDBA-47C8B32E2449}"/>
+    <workbookView xWindow="852" yWindow="-108" windowWidth="22296" windowHeight="13176" activeTab="2" xr2:uid="{F0408D6B-1B69-4349-BDBA-47C8B32E2449}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -716,7 +717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BEC1720-BBF1-4872-B6FD-32647EC01B4F}">
   <dimension ref="A2:AN41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="Y15" sqref="A2:AN41"/>
     </sheetView>
   </sheetViews>
@@ -5606,4 +5607,724 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC36086-1B63-4D1B-A8A9-186E92F2207F}">
+  <dimension ref="B2:P16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="B2:P16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
letter A in 20 by 20 lasers
</commit_message>
<xml_diff>
--- a/Green Function Method/pattern_code_far_field.xlsx
+++ b/Green Function Method/pattern_code_far_field.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Non-Hermitian Gauge Field\non-hermitian-gauge-field\Green Function Method\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89E43DB-B7B0-442D-A7E0-720C8D0703B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926504BB-30B7-43E6-8387-4B257402AD42}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="852" yWindow="-108" windowWidth="22296" windowHeight="13176" activeTab="2" xr2:uid="{F0408D6B-1B69-4349-BDBA-47C8B32E2449}"/>
   </bookViews>
@@ -5611,673 +5611,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC36086-1B63-4D1B-A8A9-186E92F2207F}">
-  <dimension ref="B2:P16"/>
+  <dimension ref="B16:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="B2:P16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="P29" sqref="P29:P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="21" width="2" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>1</v>
-      </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>0</v>
       </c>
@@ -6321,6 +5666,1199 @@
         <v>0</v>
       </c>
       <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="P28">
+        <v>1</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>1</v>
+      </c>
+      <c r="Q29">
+        <v>1</v>
+      </c>
+      <c r="R29">
+        <v>0</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>1</v>
+      </c>
+      <c r="Q30">
+        <v>1</v>
+      </c>
+      <c r="R30">
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>1</v>
+      </c>
+      <c r="Q31">
+        <v>1</v>
+      </c>
+      <c r="R31">
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>1</v>
+      </c>
+      <c r="Q32">
+        <v>1</v>
+      </c>
+      <c r="R32">
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <v>0</v>
+      </c>
+      <c r="T33">
+        <v>0</v>
+      </c>
+      <c r="U33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <v>0</v>
+      </c>
+      <c r="T34">
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <v>0</v>
+      </c>
+      <c r="T35">
+        <v>0</v>
+      </c>
+      <c r="U35">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
letter A B C
</commit_message>
<xml_diff>
--- a/Green Function Method/pattern_code_far_field.xlsx
+++ b/Green Function Method/pattern_code_far_field.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Non-Hermitian Gauge Field\non-hermitian-gauge-field\Green Function Method\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926504BB-30B7-43E6-8387-4B257402AD42}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEAE4ACE-0BA0-4A97-B724-DE011E4BA27C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="852" yWindow="-108" windowWidth="22296" windowHeight="13176" activeTab="2" xr2:uid="{F0408D6B-1B69-4349-BDBA-47C8B32E2449}"/>
   </bookViews>
@@ -30,6 +30,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5611,10 +5615,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC36086-1B63-4D1B-A8A9-186E92F2207F}">
-  <dimension ref="B16:U35"/>
+  <dimension ref="B16:U79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29:P32"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="V77" sqref="V77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6862,7 +6866,2488 @@
         <v>0</v>
       </c>
     </row>
+    <row r="38" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <v>0</v>
+      </c>
+      <c r="Q38">
+        <v>0</v>
+      </c>
+      <c r="R38">
+        <v>0</v>
+      </c>
+      <c r="S38">
+        <v>0</v>
+      </c>
+      <c r="T38">
+        <v>0</v>
+      </c>
+      <c r="U38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
+      </c>
+      <c r="Q39">
+        <v>0</v>
+      </c>
+      <c r="R39">
+        <v>0</v>
+      </c>
+      <c r="S39">
+        <v>0</v>
+      </c>
+      <c r="T39">
+        <v>0</v>
+      </c>
+      <c r="U39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <v>0</v>
+      </c>
+      <c r="Q40">
+        <v>0</v>
+      </c>
+      <c r="R40">
+        <v>0</v>
+      </c>
+      <c r="S40">
+        <v>0</v>
+      </c>
+      <c r="T40">
+        <v>0</v>
+      </c>
+      <c r="U40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+      <c r="N41">
+        <v>1</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
+      <c r="Q41">
+        <v>0</v>
+      </c>
+      <c r="R41">
+        <v>0</v>
+      </c>
+      <c r="S41">
+        <v>0</v>
+      </c>
+      <c r="T41">
+        <v>0</v>
+      </c>
+      <c r="U41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <v>1</v>
+      </c>
+      <c r="O42">
+        <v>1</v>
+      </c>
+      <c r="P42">
+        <v>0</v>
+      </c>
+      <c r="Q42">
+        <v>0</v>
+      </c>
+      <c r="R42">
+        <v>0</v>
+      </c>
+      <c r="S42">
+        <v>0</v>
+      </c>
+      <c r="T42">
+        <v>0</v>
+      </c>
+      <c r="U42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <v>1</v>
+      </c>
+      <c r="P43">
+        <v>1</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+      <c r="R43">
+        <v>0</v>
+      </c>
+      <c r="S43">
+        <v>0</v>
+      </c>
+      <c r="T43">
+        <v>0</v>
+      </c>
+      <c r="U43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>1</v>
+      </c>
+      <c r="P44">
+        <v>1</v>
+      </c>
+      <c r="Q44">
+        <v>0</v>
+      </c>
+      <c r="R44">
+        <v>0</v>
+      </c>
+      <c r="S44">
+        <v>0</v>
+      </c>
+      <c r="T44">
+        <v>0</v>
+      </c>
+      <c r="U44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>1</v>
+      </c>
+      <c r="P45">
+        <v>1</v>
+      </c>
+      <c r="Q45">
+        <v>0</v>
+      </c>
+      <c r="R45">
+        <v>0</v>
+      </c>
+      <c r="S45">
+        <v>0</v>
+      </c>
+      <c r="T45">
+        <v>0</v>
+      </c>
+      <c r="U45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <v>1</v>
+      </c>
+      <c r="P46">
+        <v>1</v>
+      </c>
+      <c r="Q46">
+        <v>0</v>
+      </c>
+      <c r="R46">
+        <v>0</v>
+      </c>
+      <c r="S46">
+        <v>0</v>
+      </c>
+      <c r="T46">
+        <v>0</v>
+      </c>
+      <c r="U46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
+      <c r="L47">
+        <v>1</v>
+      </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>1</v>
+      </c>
+      <c r="O47">
+        <v>1</v>
+      </c>
+      <c r="P47">
+        <v>0</v>
+      </c>
+      <c r="Q47">
+        <v>0</v>
+      </c>
+      <c r="R47">
+        <v>0</v>
+      </c>
+      <c r="S47">
+        <v>0</v>
+      </c>
+      <c r="T47">
+        <v>0</v>
+      </c>
+      <c r="U47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+      <c r="L48">
+        <v>1</v>
+      </c>
+      <c r="M48">
+        <v>1</v>
+      </c>
+      <c r="N48">
+        <v>1</v>
+      </c>
+      <c r="O48">
+        <v>1</v>
+      </c>
+      <c r="P48">
+        <v>0</v>
+      </c>
+      <c r="Q48">
+        <v>0</v>
+      </c>
+      <c r="R48">
+        <v>0</v>
+      </c>
+      <c r="S48">
+        <v>0</v>
+      </c>
+      <c r="T48">
+        <v>0</v>
+      </c>
+      <c r="U48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
+      <c r="O49">
+        <v>1</v>
+      </c>
+      <c r="P49">
+        <v>1</v>
+      </c>
+      <c r="Q49">
+        <v>0</v>
+      </c>
+      <c r="R49">
+        <v>0</v>
+      </c>
+      <c r="S49">
+        <v>0</v>
+      </c>
+      <c r="T49">
+        <v>0</v>
+      </c>
+      <c r="U49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50">
+        <v>0</v>
+      </c>
+      <c r="N50">
+        <v>0</v>
+      </c>
+      <c r="O50">
+        <v>1</v>
+      </c>
+      <c r="P50">
+        <v>1</v>
+      </c>
+      <c r="Q50">
+        <v>0</v>
+      </c>
+      <c r="R50">
+        <v>0</v>
+      </c>
+      <c r="S50">
+        <v>0</v>
+      </c>
+      <c r="T50">
+        <v>0</v>
+      </c>
+      <c r="U50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <v>0</v>
+      </c>
+      <c r="O51">
+        <v>1</v>
+      </c>
+      <c r="P51">
+        <v>1</v>
+      </c>
+      <c r="Q51">
+        <v>0</v>
+      </c>
+      <c r="R51">
+        <v>0</v>
+      </c>
+      <c r="S51">
+        <v>0</v>
+      </c>
+      <c r="T51">
+        <v>0</v>
+      </c>
+      <c r="U51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+      <c r="M52">
+        <v>0</v>
+      </c>
+      <c r="N52">
+        <v>0</v>
+      </c>
+      <c r="O52">
+        <v>1</v>
+      </c>
+      <c r="P52">
+        <v>1</v>
+      </c>
+      <c r="Q52">
+        <v>0</v>
+      </c>
+      <c r="R52">
+        <v>0</v>
+      </c>
+      <c r="S52">
+        <v>0</v>
+      </c>
+      <c r="T52">
+        <v>0</v>
+      </c>
+      <c r="U52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="K53">
+        <v>1</v>
+      </c>
+      <c r="L53">
+        <v>1</v>
+      </c>
+      <c r="M53">
+        <v>1</v>
+      </c>
+      <c r="N53">
+        <v>1</v>
+      </c>
+      <c r="O53">
+        <v>1</v>
+      </c>
+      <c r="P53">
+        <v>0</v>
+      </c>
+      <c r="Q53">
+        <v>0</v>
+      </c>
+      <c r="R53">
+        <v>0</v>
+      </c>
+      <c r="S53">
+        <v>0</v>
+      </c>
+      <c r="T53">
+        <v>0</v>
+      </c>
+      <c r="U53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="J54">
+        <v>1</v>
+      </c>
+      <c r="K54">
+        <v>1</v>
+      </c>
+      <c r="L54">
+        <v>1</v>
+      </c>
+      <c r="M54">
+        <v>1</v>
+      </c>
+      <c r="N54">
+        <v>1</v>
+      </c>
+      <c r="O54">
+        <v>0</v>
+      </c>
+      <c r="P54">
+        <v>0</v>
+      </c>
+      <c r="Q54">
+        <v>0</v>
+      </c>
+      <c r="R54">
+        <v>0</v>
+      </c>
+      <c r="S54">
+        <v>0</v>
+      </c>
+      <c r="T54">
+        <v>0</v>
+      </c>
+      <c r="U54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+      <c r="N55">
+        <v>0</v>
+      </c>
+      <c r="O55">
+        <v>0</v>
+      </c>
+      <c r="P55">
+        <v>0</v>
+      </c>
+      <c r="Q55">
+        <v>0</v>
+      </c>
+      <c r="R55">
+        <v>0</v>
+      </c>
+      <c r="S55">
+        <v>0</v>
+      </c>
+      <c r="T55">
+        <v>0</v>
+      </c>
+      <c r="U55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
+      <c r="M56">
+        <v>0</v>
+      </c>
+      <c r="N56">
+        <v>0</v>
+      </c>
+      <c r="O56">
+        <v>0</v>
+      </c>
+      <c r="P56">
+        <v>0</v>
+      </c>
+      <c r="Q56">
+        <v>0</v>
+      </c>
+      <c r="R56">
+        <v>0</v>
+      </c>
+      <c r="S56">
+        <v>0</v>
+      </c>
+      <c r="T56">
+        <v>0</v>
+      </c>
+      <c r="U56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
+      <c r="M57">
+        <v>0</v>
+      </c>
+      <c r="N57">
+        <v>0</v>
+      </c>
+      <c r="O57">
+        <v>0</v>
+      </c>
+      <c r="P57">
+        <v>0</v>
+      </c>
+      <c r="Q57">
+        <v>0</v>
+      </c>
+      <c r="R57">
+        <v>0</v>
+      </c>
+      <c r="S57">
+        <v>0</v>
+      </c>
+      <c r="T57">
+        <v>0</v>
+      </c>
+      <c r="U57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>0</v>
+      </c>
+      <c r="L60">
+        <v>0</v>
+      </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+      <c r="N60">
+        <v>0</v>
+      </c>
+      <c r="O60">
+        <v>0</v>
+      </c>
+      <c r="P60">
+        <v>0</v>
+      </c>
+      <c r="Q60">
+        <v>0</v>
+      </c>
+      <c r="R60">
+        <v>0</v>
+      </c>
+      <c r="S60">
+        <v>0</v>
+      </c>
+      <c r="T60">
+        <v>0</v>
+      </c>
+      <c r="U60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="K61">
+        <v>0</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+      <c r="M61">
+        <v>0</v>
+      </c>
+      <c r="N61">
+        <v>0</v>
+      </c>
+      <c r="O61">
+        <v>0</v>
+      </c>
+      <c r="P61">
+        <v>0</v>
+      </c>
+      <c r="Q61">
+        <v>0</v>
+      </c>
+      <c r="R61">
+        <v>0</v>
+      </c>
+      <c r="S61">
+        <v>0</v>
+      </c>
+      <c r="T61">
+        <v>0</v>
+      </c>
+      <c r="U61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <v>0</v>
+      </c>
+      <c r="L62">
+        <v>0</v>
+      </c>
+      <c r="M62">
+        <v>0</v>
+      </c>
+      <c r="N62">
+        <v>0</v>
+      </c>
+      <c r="O62">
+        <v>0</v>
+      </c>
+      <c r="P62">
+        <v>0</v>
+      </c>
+      <c r="Q62">
+        <v>0</v>
+      </c>
+      <c r="R62">
+        <v>0</v>
+      </c>
+      <c r="S62">
+        <v>0</v>
+      </c>
+      <c r="T62">
+        <v>0</v>
+      </c>
+      <c r="U62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
+      <c r="I63">
+        <v>1</v>
+      </c>
+      <c r="J63">
+        <v>1</v>
+      </c>
+      <c r="K63">
+        <v>1</v>
+      </c>
+      <c r="L63">
+        <v>1</v>
+      </c>
+      <c r="M63">
+        <v>1</v>
+      </c>
+      <c r="N63">
+        <v>1</v>
+      </c>
+      <c r="O63">
+        <v>0</v>
+      </c>
+      <c r="P63">
+        <v>0</v>
+      </c>
+      <c r="Q63">
+        <v>0</v>
+      </c>
+      <c r="R63">
+        <v>0</v>
+      </c>
+      <c r="S63">
+        <v>0</v>
+      </c>
+      <c r="T63">
+        <v>0</v>
+      </c>
+      <c r="U63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <v>1</v>
+      </c>
+      <c r="J64">
+        <v>1</v>
+      </c>
+      <c r="K64">
+        <v>1</v>
+      </c>
+      <c r="L64">
+        <v>1</v>
+      </c>
+      <c r="M64">
+        <v>1</v>
+      </c>
+      <c r="N64">
+        <v>1</v>
+      </c>
+      <c r="O64">
+        <v>1</v>
+      </c>
+      <c r="P64">
+        <v>0</v>
+      </c>
+      <c r="Q64">
+        <v>0</v>
+      </c>
+      <c r="R64">
+        <v>0</v>
+      </c>
+      <c r="S64">
+        <v>0</v>
+      </c>
+      <c r="T64">
+        <v>0</v>
+      </c>
+      <c r="U64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65">
+        <v>0</v>
+      </c>
+      <c r="M65">
+        <v>0</v>
+      </c>
+      <c r="N65">
+        <v>0</v>
+      </c>
+      <c r="O65">
+        <v>1</v>
+      </c>
+      <c r="P65">
+        <v>1</v>
+      </c>
+      <c r="Q65">
+        <v>0</v>
+      </c>
+      <c r="R65">
+        <v>0</v>
+      </c>
+      <c r="S65">
+        <v>0</v>
+      </c>
+      <c r="T65">
+        <v>0</v>
+      </c>
+      <c r="U65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66">
+        <v>1</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
+      <c r="M66">
+        <v>0</v>
+      </c>
+      <c r="N66">
+        <v>0</v>
+      </c>
+      <c r="O66">
+        <v>1</v>
+      </c>
+      <c r="P66">
+        <v>1</v>
+      </c>
+      <c r="Q66">
+        <v>0</v>
+      </c>
+      <c r="R66">
+        <v>0</v>
+      </c>
+      <c r="S66">
+        <v>0</v>
+      </c>
+      <c r="T66">
+        <v>0</v>
+      </c>
+      <c r="U66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67">
+        <v>1</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <v>0</v>
+      </c>
+      <c r="L67">
+        <v>0</v>
+      </c>
+      <c r="M67">
+        <v>0</v>
+      </c>
+      <c r="N67">
+        <v>0</v>
+      </c>
+      <c r="O67">
+        <v>0</v>
+      </c>
+      <c r="P67">
+        <v>0</v>
+      </c>
+      <c r="Q67">
+        <v>0</v>
+      </c>
+      <c r="R67">
+        <v>0</v>
+      </c>
+      <c r="S67">
+        <v>0</v>
+      </c>
+      <c r="T67">
+        <v>0</v>
+      </c>
+      <c r="U67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+      <c r="J68">
+        <v>0</v>
+      </c>
+      <c r="K68">
+        <v>0</v>
+      </c>
+      <c r="L68">
+        <v>0</v>
+      </c>
+      <c r="M68">
+        <v>0</v>
+      </c>
+      <c r="N68">
+        <v>0</v>
+      </c>
+      <c r="O68">
+        <v>0</v>
+      </c>
+      <c r="P68">
+        <v>0</v>
+      </c>
+      <c r="Q68">
+        <v>0</v>
+      </c>
+      <c r="R68">
+        <v>0</v>
+      </c>
+      <c r="S68">
+        <v>0</v>
+      </c>
+      <c r="T68">
+        <v>0</v>
+      </c>
+      <c r="U68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69">
+        <v>1</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+      <c r="K69">
+        <v>0</v>
+      </c>
+      <c r="L69">
+        <v>0</v>
+      </c>
+      <c r="M69">
+        <v>0</v>
+      </c>
+      <c r="N69">
+        <v>0</v>
+      </c>
+      <c r="O69">
+        <v>0</v>
+      </c>
+      <c r="P69">
+        <v>0</v>
+      </c>
+      <c r="Q69">
+        <v>0</v>
+      </c>
+      <c r="R69">
+        <v>0</v>
+      </c>
+      <c r="S69">
+        <v>0</v>
+      </c>
+      <c r="T69">
+        <v>0</v>
+      </c>
+      <c r="U69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70">
+        <v>1</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
+      <c r="K70">
+        <v>0</v>
+      </c>
+      <c r="L70">
+        <v>0</v>
+      </c>
+      <c r="M70">
+        <v>0</v>
+      </c>
+      <c r="N70">
+        <v>0</v>
+      </c>
+      <c r="O70">
+        <v>0</v>
+      </c>
+      <c r="P70">
+        <v>0</v>
+      </c>
+      <c r="Q70">
+        <v>0</v>
+      </c>
+      <c r="R70">
+        <v>0</v>
+      </c>
+      <c r="S70">
+        <v>0</v>
+      </c>
+      <c r="T70">
+        <v>0</v>
+      </c>
+      <c r="U70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <v>1</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+      <c r="K71">
+        <v>0</v>
+      </c>
+      <c r="L71">
+        <v>0</v>
+      </c>
+      <c r="M71">
+        <v>0</v>
+      </c>
+      <c r="N71">
+        <v>0</v>
+      </c>
+      <c r="O71">
+        <v>0</v>
+      </c>
+      <c r="P71">
+        <v>0</v>
+      </c>
+      <c r="Q71">
+        <v>0</v>
+      </c>
+      <c r="R71">
+        <v>0</v>
+      </c>
+      <c r="S71">
+        <v>0</v>
+      </c>
+      <c r="T71">
+        <v>0</v>
+      </c>
+      <c r="U71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72">
+        <v>1</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+      <c r="K72">
+        <v>0</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+      <c r="M72">
+        <v>0</v>
+      </c>
+      <c r="N72">
+        <v>0</v>
+      </c>
+      <c r="O72">
+        <v>0</v>
+      </c>
+      <c r="P72">
+        <v>0</v>
+      </c>
+      <c r="Q72">
+        <v>0</v>
+      </c>
+      <c r="R72">
+        <v>0</v>
+      </c>
+      <c r="S72">
+        <v>0</v>
+      </c>
+      <c r="T72">
+        <v>0</v>
+      </c>
+      <c r="U72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73">
+        <v>1</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+      <c r="K73">
+        <v>0</v>
+      </c>
+      <c r="L73">
+        <v>0</v>
+      </c>
+      <c r="M73">
+        <v>0</v>
+      </c>
+      <c r="N73">
+        <v>0</v>
+      </c>
+      <c r="O73">
+        <v>0</v>
+      </c>
+      <c r="P73">
+        <v>0</v>
+      </c>
+      <c r="Q73">
+        <v>0</v>
+      </c>
+      <c r="R73">
+        <v>0</v>
+      </c>
+      <c r="S73">
+        <v>0</v>
+      </c>
+      <c r="T73">
+        <v>0</v>
+      </c>
+      <c r="U73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>1</v>
+      </c>
+      <c r="G74">
+        <v>1</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+      <c r="J74">
+        <v>0</v>
+      </c>
+      <c r="K74">
+        <v>0</v>
+      </c>
+      <c r="L74">
+        <v>0</v>
+      </c>
+      <c r="M74">
+        <v>0</v>
+      </c>
+      <c r="N74">
+        <v>0</v>
+      </c>
+      <c r="O74">
+        <v>1</v>
+      </c>
+      <c r="P74">
+        <v>1</v>
+      </c>
+      <c r="Q74">
+        <v>0</v>
+      </c>
+      <c r="R74">
+        <v>0</v>
+      </c>
+      <c r="S74">
+        <v>0</v>
+      </c>
+      <c r="T74">
+        <v>0</v>
+      </c>
+      <c r="U74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>1</v>
+      </c>
+      <c r="H75">
+        <v>1</v>
+      </c>
+      <c r="I75">
+        <v>1</v>
+      </c>
+      <c r="J75">
+        <v>1</v>
+      </c>
+      <c r="K75">
+        <v>1</v>
+      </c>
+      <c r="L75">
+        <v>1</v>
+      </c>
+      <c r="M75">
+        <v>1</v>
+      </c>
+      <c r="N75">
+        <v>1</v>
+      </c>
+      <c r="O75">
+        <v>1</v>
+      </c>
+      <c r="P75">
+        <v>0</v>
+      </c>
+      <c r="Q75">
+        <v>0</v>
+      </c>
+      <c r="R75">
+        <v>0</v>
+      </c>
+      <c r="S75">
+        <v>0</v>
+      </c>
+      <c r="T75">
+        <v>0</v>
+      </c>
+      <c r="U75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>1</v>
+      </c>
+      <c r="I76">
+        <v>1</v>
+      </c>
+      <c r="J76">
+        <v>1</v>
+      </c>
+      <c r="K76">
+        <v>1</v>
+      </c>
+      <c r="L76">
+        <v>1</v>
+      </c>
+      <c r="M76">
+        <v>1</v>
+      </c>
+      <c r="N76">
+        <v>1</v>
+      </c>
+      <c r="O76">
+        <v>0</v>
+      </c>
+      <c r="P76">
+        <v>0</v>
+      </c>
+      <c r="Q76">
+        <v>0</v>
+      </c>
+      <c r="R76">
+        <v>0</v>
+      </c>
+      <c r="S76">
+        <v>0</v>
+      </c>
+      <c r="T76">
+        <v>0</v>
+      </c>
+      <c r="U76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="J77">
+        <v>0</v>
+      </c>
+      <c r="K77">
+        <v>0</v>
+      </c>
+      <c r="L77">
+        <v>0</v>
+      </c>
+      <c r="M77">
+        <v>0</v>
+      </c>
+      <c r="N77">
+        <v>0</v>
+      </c>
+      <c r="O77">
+        <v>0</v>
+      </c>
+      <c r="P77">
+        <v>0</v>
+      </c>
+      <c r="Q77">
+        <v>0</v>
+      </c>
+      <c r="R77">
+        <v>0</v>
+      </c>
+      <c r="S77">
+        <v>0</v>
+      </c>
+      <c r="T77">
+        <v>0</v>
+      </c>
+      <c r="U77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="I78">
+        <v>0</v>
+      </c>
+      <c r="J78">
+        <v>0</v>
+      </c>
+      <c r="K78">
+        <v>0</v>
+      </c>
+      <c r="L78">
+        <v>0</v>
+      </c>
+      <c r="M78">
+        <v>0</v>
+      </c>
+      <c r="N78">
+        <v>0</v>
+      </c>
+      <c r="O78">
+        <v>0</v>
+      </c>
+      <c r="P78">
+        <v>0</v>
+      </c>
+      <c r="Q78">
+        <v>0</v>
+      </c>
+      <c r="R78">
+        <v>0</v>
+      </c>
+      <c r="S78">
+        <v>0</v>
+      </c>
+      <c r="T78">
+        <v>0</v>
+      </c>
+      <c r="U78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79">
+        <v>0</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+      <c r="K79">
+        <v>0</v>
+      </c>
+      <c r="L79">
+        <v>0</v>
+      </c>
+      <c r="M79">
+        <v>0</v>
+      </c>
+      <c r="N79">
+        <v>0</v>
+      </c>
+      <c r="O79">
+        <v>0</v>
+      </c>
+      <c r="P79">
+        <v>0</v>
+      </c>
+      <c r="Q79">
+        <v>0</v>
+      </c>
+      <c r="R79">
+        <v>0</v>
+      </c>
+      <c r="S79">
+        <v>0</v>
+      </c>
+      <c r="T79">
+        <v>0</v>
+      </c>
+      <c r="U79">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
backward calculation errors fixed
</commit_message>
<xml_diff>
--- a/Green Function Method/pattern_code_far_field.xlsx
+++ b/Green Function Method/pattern_code_far_field.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Non-Hermitian Gauge Field\non-hermitian-gauge-field\Green Function Method\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03F422F-B3DA-4E7E-B5EF-94EC3770BF56}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE261CD-E368-4707-A352-2F0A9A6F585E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="852" yWindow="-108" windowWidth="22296" windowHeight="13176" xr2:uid="{F0408D6B-1B69-4349-BDBA-47C8B32E2449}"/>
   </bookViews>
@@ -94,6 +94,82 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>97</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2F54215-7659-4621-9911-B47971B379B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5581650" y="9486900"/>
+          <a:ext cx="15354300" cy="16802100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="100000"/>
+            <a:t>A</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -395,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{139E4D90-05E5-4074-BB79-3C52273E58F6}">
   <dimension ref="B2:CC81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:CC81"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="CY83" sqref="CY83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19767,6 +19843,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -29592,8 +29669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC36086-1B63-4D1B-A8A9-186E92F2207F}">
   <dimension ref="B16:U79"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="V77" sqref="V77"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="W51" sqref="W51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>